<commit_message>
Updating wy2016-2017 wwTHg model results; Adding to Spillway, wy2016-2017: a new wwTHg folder (three models); and updated Q and WQ worksheet.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwTHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwTHg Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CB69CA56-0942-4F70-B843-277B203E94B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A0FAFF1A-D5C0-4ABC-B097-7932ECCEB81E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="487">
   <si>
     <t>Model #</t>
   </si>
@@ -918,6 +918,573 @@
   </si>
   <si>
     <t xml:space="preserve">  E: 0.232</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym1 &lt;- loadReg(wwTHg ~model(1), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 23</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.639</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 6.6765</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Period of record: 2016-01-24 to 2017-04-04</t>
+  </si>
+  <si>
+    <t>(Intercept)   -2.687     0.2146  -12.52       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.418     0.1025   13.83       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7176</t>
+  </si>
+  <si>
+    <t>R-squared: 90.1 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 53.2 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0045</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0876</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min  25%  50%  75%  90%  95%  Max</t>
+  </si>
+  <si>
+    <t>Est   0 0.42 0.85 3.49 4.73 5.19 5.36</t>
+  </si>
+  <si>
+    <t>Obs   0 0.07 0.50 3.38 5.04 5.64 8.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -7.423 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8284</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym2 &lt;- loadReg(wwTHg ~model(2), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym2</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.2920    0.31010 -10.616  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4176    0.09182  15.438  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1381    0.05552   2.486  0.0128</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.5756</t>
+  </si>
+  <si>
+    <t>R-squared: 92.44 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 59.39 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9595</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0661</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min  25% 50%  75%  90%  95%  Max</t>
+  </si>
+  <si>
+    <t>Est   0 0.25 0.6 4.33 6.84 7.86 8.25</t>
+  </si>
+  <si>
+    <t>Obs   0 0.07 0.5 3.38 5.04 5.64 8.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 14.79 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7781</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym3 &lt;- loadReg(wwTHg ~model(3), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            Estimate Std. Error  z-score p-value</t>
+  </si>
+  <si>
+    <t>(Intercept)  -2.6716     0.2212 -12.0777   0.000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4348     0.1109  12.9431   0.000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.2122     0.4550  -0.4663   0.618</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7454</t>
+  </si>
+  <si>
+    <t>R-squared: 90.21 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 53.44 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9378</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0119</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.058</t>
+  </si>
+  <si>
+    <t>lnQ     1.126</t>
+  </si>
+  <si>
+    <t>DECTIME 1.126</t>
+  </si>
+  <si>
+    <t>Est   0 0.47 0.83 3.42 4.70 5.01 5.32</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -8.735 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8244</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym4 &lt;- loadReg(wwTHg ~model(4), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -0.7406     2.3529 -0.3148  0.7294</t>
+  </si>
+  <si>
+    <t>lnQ           1.4259     0.1245 11.4505  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.8812     1.8932 -0.9937  0.2804</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -1.2885     1.9932 -0.6465  0.4793</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7179</t>
+  </si>
+  <si>
+    <t>R-squared: 91.04 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 55.49 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0046</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               VIF</t>
+  </si>
+  <si>
+    <t>lnQ          1.475</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 11.839</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.239</t>
+  </si>
+  <si>
+    <t>Est   0 0.34 0.75 3.26 3.87 6.83 7.42</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -3.179 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8793</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym5 &lt;- loadReg(wwTHg ~model(5), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym5</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.4911    0.30025 -11.627  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4908    0.09119  16.349  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1983    0.05834   3.399  0.0009</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.9005    0.42014  -2.143  0.0256</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.4879</t>
+  </si>
+  <si>
+    <t>R-squared: 93.91 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 64.37 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9781</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.3394</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.0604</t>
+  </si>
+  <si>
+    <t>lnQ     1.163</t>
+  </si>
+  <si>
+    <t>lnQ2    1.303</t>
+  </si>
+  <si>
+    <t>DECTIME 1.466</t>
+  </si>
+  <si>
+    <t>Est   0 0.27 0.47 4.18 7.40 7.87 9.21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 14.85 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7482</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym6 &lt;- loadReg(wwTHg ~model(6), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym6</t>
+  </si>
+  <si>
+    <t>(Intercept)  -1.7365    2.20066 -0.7891  0.3765</t>
+  </si>
+  <si>
+    <t>lnQ           1.4278    0.11391 12.5341  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1257    0.05792  2.1698  0.0208</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -1.4215    1.74469 -0.8148  0.3614</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -1.0253    1.82724 -0.5611  0.5277</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.6007</t>
+  </si>
+  <si>
+    <t>R-squared: 92.9 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 60.83 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1289</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.2685</t>
+  </si>
+  <si>
+    <t>lnQ2         1.043</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 12.016</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min  25%  50%  75%  90%  95%   Max</t>
+  </si>
+  <si>
+    <t>Est   0 0.23 0.53 4.45 5.92 8.71 10.10</t>
+  </si>
+  <si>
+    <t>Obs   0 0.07 0.50 3.38 5.04 5.64  8.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 15.96 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.7856</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym7 &lt;- loadReg(wwTHg ~model(7), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym7</t>
+  </si>
+  <si>
+    <t>(Intercept)   0.1438     2.3994  0.05993  0.9460</t>
+  </si>
+  <si>
+    <t>lnQ           1.4790     0.1284 11.52258  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.6654     0.4986 -1.33450  0.1407</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -2.7264     1.9606 -1.39059  0.1255</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -1.8031     1.9911 -0.90558  0.3114</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.6895</t>
+  </si>
+  <si>
+    <t>R-squared: 91.85 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 57.66 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.1712</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.1055</t>
+  </si>
+  <si>
+    <t>lnQ          1.631</t>
+  </si>
+  <si>
+    <t>DECTIME      1.461</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 13.218</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.755</t>
+  </si>
+  <si>
+    <t>Est   0 0.38 0.83 2.56 3.69 7.75 8.22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -5.537 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8161</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym8 &lt;- loadReg(wwTHg ~model(8), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym8</t>
+  </si>
+  <si>
+    <t>(Intercept)  -0.4958    1.79094 -0.2768  0.7477</t>
+  </si>
+  <si>
+    <t>lnQ           1.5404    0.09667 15.9337  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.2036    0.05160  3.9464  0.0001</t>
+  </si>
+  <si>
+    <t>DECTIME      -1.3983    0.41458 -3.3727  0.0006</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -2.9123    1.45819 -1.9972  0.0277</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -1.9433    1.48057 -1.3126  0.1362</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.381</t>
+  </si>
+  <si>
+    <t>R-squared: 95.75 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 72.62 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9858</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.6418</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.4131</t>
+  </si>
+  <si>
+    <t>lnQ          1.674</t>
+  </si>
+  <si>
+    <t>lnQ2         1.305</t>
+  </si>
+  <si>
+    <t>DECTIME      1.828</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 13.232</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 13.763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min  25%  50%  75%  90%   95%   Max</t>
+  </si>
+  <si>
+    <t>Est   0 0.18 0.61 3.35 4.47 12.90 14.90</t>
+  </si>
+  <si>
+    <t>Obs   0 0.07 0.50 3.38 5.04  5.64  8.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 23.83 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.1216</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym9 &lt;- loadReg(wwTHg ~model(9), data = wwTHg_Spillway, flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Spillwaym9</t>
+  </si>
+  <si>
+    <t>(Intercept)  -0.8469    1.58473 -0.5344  0.5235</t>
+  </si>
+  <si>
+    <t>lnQ           1.3325    0.12077 11.0338  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.2693    0.05291  5.0902  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.9192    0.41520 -2.2138  0.0132</t>
+  </si>
+  <si>
+    <t>DECTIME2     -9.2658    3.81650 -2.4278  0.0072</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.6902    1.57755 -0.4375  0.6009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  -0.6919    1.40277 -0.4933  0.5558</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.2959</t>
+  </si>
+  <si>
+    <t>R-squared: 96.89 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 79.83 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9638</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0955</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: -0.3173</t>
+  </si>
+  <si>
+    <t>lnQ          3.365</t>
+  </si>
+  <si>
+    <t>lnQ2         1.767</t>
+  </si>
+  <si>
+    <t>DECTIME      2.361</t>
+  </si>
+  <si>
+    <t>DECTIME2     4.110</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 19.946</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 15.911</t>
+  </si>
+  <si>
+    <t>Est   0 0.19 0.56 3.62 4.65 12.00 14.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 21.89 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.2387</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 23; Period of record: 2016-01-24 to 2017-04-04</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1237,15 +1804,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1267,21 +1825,23 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1459,116 +2019,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2036,13 +2486,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
-    <tabColor theme="5" tint="0.59999389629810485"/>
+    <tabColor rgb="FFFFFFC1"/>
   </sheetPr>
   <dimension ref="A1:AI68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2056,10 +2506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="34"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>21</v>
@@ -2098,24 +2548,24 @@
       <c r="L2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="35"/>
+      <c r="O2" s="32"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="40"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="37"/>
       <c r="Z4" s="18" t="s">
         <v>51</v>
       </c>
@@ -2130,21 +2580,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="30" t="s">
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="30"/>
+      <c r="L5" s="41"/>
       <c r="Z5" s="18" t="s">
         <v>52</v>
       </c>
@@ -2640,34 +3090,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="37"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="31"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="30" t="s">
+      <c r="B18" s="38" t="s">
+        <v>486</v>
+      </c>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="30"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -2714,35 +3166,45 @@
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A20" s="29">
+      <c r="A20" s="11">
         <v>1</v>
       </c>
       <c r="B20" s="11">
         <v>0</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
+      <c r="I20" s="11">
+        <v>90.1</v>
+      </c>
+      <c r="J20" s="11">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="K20" s="11">
+        <v>-7.423</v>
+      </c>
+      <c r="L20" s="30">
+        <v>0.82840000000000003</v>
+      </c>
+      <c r="M20" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N20" s="8" t="s">
         <v>17</v>
       </c>
@@ -2754,33 +3216,45 @@
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A21" s="29">
+      <c r="A21" s="11">
         <v>2</v>
       </c>
       <c r="B21" s="11">
         <v>0</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="10" t="s">
+      <c r="C21" s="28">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="D21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
+      <c r="I21" s="11">
+        <v>92.44</v>
+      </c>
+      <c r="J21" s="11">
+        <v>0.3276</v>
+      </c>
+      <c r="K21" s="11">
+        <v>14.79</v>
+      </c>
+      <c r="L21" s="30">
+        <v>0.77810000000000001</v>
+      </c>
+      <c r="M21" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N21" s="8" t="s">
         <v>17</v>
       </c>
@@ -2795,13 +3269,15 @@
       <c r="A22" s="29">
         <v>3</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="6">
         <v>0</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="23"/>
+      <c r="D22" s="23">
+        <v>0.61799999999999999</v>
+      </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
       </c>
@@ -2811,13 +3287,21 @@
       <c r="G22" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="H22" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="I22" s="30">
+        <v>90.21</v>
+      </c>
+      <c r="J22" s="30">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="K22" s="30">
+        <v>-8.7349999999999994</v>
+      </c>
+      <c r="L22" s="30">
+        <v>0.82440000000000002</v>
+      </c>
       <c r="M22" s="29"/>
       <c r="N22" s="8" t="s">
         <v>17</v>
@@ -2833,7 +3317,7 @@
       <c r="A23" s="29">
         <v>4</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="6">
         <v>0</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2845,15 +3329,27 @@
       <c r="E23" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="11" t="s">
+      <c r="F23" s="6">
+        <v>0.82440000000000002</v>
+      </c>
+      <c r="G23" s="30">
+        <v>0.4793</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="I23" s="30">
+        <v>91.04</v>
+      </c>
+      <c r="J23" s="30">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="K23" s="30">
+        <v>-3.1789999999999998</v>
+      </c>
+      <c r="L23" s="30">
+        <v>0.87929999999999997</v>
+      </c>
       <c r="M23" s="29"/>
       <c r="N23" s="8" t="s">
         <v>17</v>
@@ -2866,31 +3362,45 @@
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A24" s="29">
+      <c r="A24" s="11">
         <v>5</v>
       </c>
       <c r="B24" s="11">
         <v>0</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="10" t="s">
+      <c r="C24" s="11">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="E24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H24" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
+      <c r="I24" s="11">
+        <v>93.91</v>
+      </c>
+      <c r="J24" s="11">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="K24" s="11">
+        <v>14.85</v>
+      </c>
+      <c r="L24" s="30">
+        <v>0.74819999999999998</v>
+      </c>
+      <c r="M24" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N24" s="8" t="s">
         <v>17</v>
       </c>
@@ -2905,25 +3415,39 @@
       <c r="A25" s="29">
         <v>6</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="6">
         <v>0</v>
       </c>
-      <c r="C25" s="29"/>
+      <c r="C25" s="30">
+        <v>2.0799999999999999E-2</v>
+      </c>
       <c r="D25" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="6"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="11" t="s">
+      <c r="F25" s="6">
+        <v>0.3614</v>
+      </c>
+      <c r="G25" s="30">
+        <v>0.52769999999999995</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="I25" s="30">
+        <v>92.9</v>
+      </c>
+      <c r="J25" s="30">
+        <v>0.26850000000000002</v>
+      </c>
+      <c r="K25" s="30">
+        <v>15.96</v>
+      </c>
+      <c r="L25" s="30">
+        <v>0.78559999999999997</v>
+      </c>
       <c r="M25" s="29"/>
       <c r="N25" s="8" t="s">
         <v>17</v>
@@ -2939,25 +3463,39 @@
       <c r="A26" s="29">
         <v>7</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="6">
         <v>0</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6">
+        <v>0.14069999999999999</v>
+      </c>
       <c r="E26" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="11" t="s">
+      <c r="F26" s="6">
+        <v>0.1255</v>
+      </c>
+      <c r="G26" s="30">
+        <v>0.31140000000000001</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
+      <c r="I26" s="30">
+        <v>91.85</v>
+      </c>
+      <c r="J26" s="30">
+        <v>-0.1055</v>
+      </c>
+      <c r="K26" s="30">
+        <v>-5.5369999999999999</v>
+      </c>
+      <c r="L26" s="30">
+        <v>0.81610000000000005</v>
+      </c>
       <c r="M26" s="29"/>
       <c r="N26" s="8" t="s">
         <v>17</v>
@@ -2973,23 +3511,39 @@
       <c r="A27" s="29">
         <v>8</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="6">
         <v>0</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="30">
+        <v>1E-4</v>
+      </c>
+      <c r="D27" s="6">
+        <v>5.9999999999999995E-4</v>
+      </c>
       <c r="E27" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="11" t="s">
+      <c r="F27" s="6">
+        <v>2.7699999999999999E-2</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.13619999999999999</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
+      <c r="I27" s="30">
+        <v>95.75</v>
+      </c>
+      <c r="J27" s="30">
+        <v>-0.41310000000000002</v>
+      </c>
+      <c r="K27" s="30">
+        <v>23.83</v>
+      </c>
+      <c r="L27" s="30">
+        <v>0.1216</v>
+      </c>
       <c r="M27" s="29"/>
       <c r="N27" s="8" t="s">
         <v>17</v>
@@ -3005,21 +3559,39 @@
       <c r="A28" s="29">
         <v>9</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="6">
         <v>0</v>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="11" t="s">
+      <c r="C28" s="30">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1.32E-2</v>
+      </c>
+      <c r="E28" s="6">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0.60089999999999999</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0.55579999999999996</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
+      <c r="I28" s="30">
+        <v>96.89</v>
+      </c>
+      <c r="J28" s="30">
+        <v>-0.31730000000000003</v>
+      </c>
+      <c r="K28" s="30">
+        <v>21.89</v>
+      </c>
+      <c r="L28" s="30">
+        <v>0.2387</v>
+      </c>
       <c r="M28" s="29"/>
       <c r="N28" s="8" t="s">
         <v>17</v>
@@ -3032,34 +3604,34 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="40"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="37"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="31"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="30" t="s">
+      <c r="B31" s="38"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="30"/>
+      <c r="L31" s="41"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -3424,34 +3996,34 @@
       </c>
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="40"/>
+      <c r="C43" s="36"/>
+      <c r="D43" s="36"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="37"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="31"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
-      <c r="I44" s="32"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="30" t="s">
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="40"/>
+      <c r="K44" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="30"/>
+      <c r="L44" s="41"/>
     </row>
     <row r="45" spans="1:27" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
@@ -3821,34 +4393,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="38" t="s">
+      <c r="B57" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="C57" s="39"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="39"/>
-      <c r="I57" s="39"/>
-      <c r="J57" s="40"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="41"/>
+      <c r="L57" s="41"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="31"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="32"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
-      <c r="I58" s="32"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="30" t="s">
+      <c r="B58" s="38"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="39"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="39"/>
+      <c r="J58" s="40"/>
+      <c r="K58" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="30"/>
+      <c r="L58" s="41"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -4088,12 +4660,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K58:L58"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B18:J18"/>
@@ -4106,129 +4672,135 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="K44:L44"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
-    <cfRule type="cellIs" dxfId="41" priority="54" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="54" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="55" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="56" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="56" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K55 K60:K1048576 K57 K29">
-    <cfRule type="cellIs" dxfId="38" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="40" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="41" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="41" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61 D62 C64:C65 D64 C67:C68 D66:D68 E68 F63:G63 F65:G68">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="37" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46:L54">
-    <cfRule type="cellIs" dxfId="35" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:K54">
-    <cfRule type="cellIs" dxfId="32" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47 D48 C50:C51 D50 C53:C54 D52:D54 E54 F49:G49 F51:G54">
-    <cfRule type="cellIs" dxfId="30" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8 D9 C11:C12 D11 C14:C15 D13:D15 E15 F10:G10 F12:G15">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33:L41">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:K41">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34 D35 C37:C38 D37 C40:C41 D39:D41 E41 F36:G36 F38:G41">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:L28">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20:K28">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21 D22 C24:C25 D24 C27:C28 D26:D28 E28 F23:G23 F25:G28">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L7:L15">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>0.8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
       <formula>0.8</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7:K15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>-25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6712,115 +7284,173 @@
   <dimension ref="A1:A529"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -6829,1477 +7459,2289 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A525" s="13"/>
+      <c r="A525" s="16"/>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A526" s="15"/>
+      <c r="A526" s="16"/>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A527" s="16"/>
+      <c r="A527" s="17"/>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A528" s="17"/>
+      <c r="A528" s="12"/>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A529" s="12"/>

</xml_diff>

<commit_message>
Updated model stats for wy2016-17 wwTHg; Added files to Combined Outflow, wy2016-17: updated Q and WQ worksheet; added rloadest wwTHg folder.
</commit_message>
<xml_diff>
--- a/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwTHg Model Results.xlsx
+++ b/2018_CCSB_LoadsData_WY2010-2017/Model Stats_rloadest/1_wy2016_2017/1_wwTHg Model Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\slrose\R\2018_CCSB_LoadsData_WY2010-2017\Model Stats_rloadest\1_wy2016_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{152030F4-259E-4618-87E8-B1D2FED3F345}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6A17CF1C-9788-4E5A-AA9A-9ACEE1A246C7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="990" yWindow="30" windowWidth="9630" windowHeight="13440" tabRatio="727" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="852">
   <si>
     <t>Model #</t>
   </si>
@@ -2043,6 +2043,543 @@
   </si>
   <si>
     <t>Number of Uncensored Observations: 29; Period of record: 2016-01-20 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm1 &lt;- loadReg(wwTHg ~model(1), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Number of Observations: 34</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           Center of Decimal Time: 2016.626</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                  Center of ln(Q): 7.0699</t>
+  </si>
+  <si>
+    <t>(Intercept)   -2.071    0.16057  -12.90       0</t>
+  </si>
+  <si>
+    <t>lnQ            1.417    0.09654   14.68       0</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8586</t>
+  </si>
+  <si>
+    <t>G-squared: 69.56 on 1 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.217</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4859</t>
+  </si>
+  <si>
+    <t>Est   0 0.05 0.68 2.23 4.73 5.89 6.07</t>
+  </si>
+  <si>
+    <t>Obs   0 0.03 0.22 1.80 4.95 5.65 8.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 5.297 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8723</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm2 &lt;- loadReg(wwTHg ~model(2), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm2</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.26187    0.25189 -8.9795   0.000</t>
+  </si>
+  <si>
+    <t>lnQ          1.41732    0.09659 14.6742   0.000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.06909    0.07014  0.9851   0.306</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.8594</t>
+  </si>
+  <si>
+    <t>R-squared: 87.46 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 70.61 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9799</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2136</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.5375</t>
+  </si>
+  <si>
+    <t>Est   0 0.04 0.59 2.27 5.52 7.16 7.42</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 16.72 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8468</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm3 &lt;- loadReg(wwTHg ~model(3), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm3</t>
+  </si>
+  <si>
+    <t>(Intercept)  -2.0586     0.1544 -13.335  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.4991     0.1021  14.686  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.6875     0.3586  -1.917  0.0509</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7923</t>
+  </si>
+  <si>
+    <t>R-squared: 88.44 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 73.37 on 2 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.7715</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4287</t>
+  </si>
+  <si>
+    <t>lnQ     1.211</t>
+  </si>
+  <si>
+    <t>DECTIME 1.211</t>
+  </si>
+  <si>
+    <t>Est   0 0.06 0.62 1.88 4.00 4.94 5.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: -4.188 percent</t>
+  </si>
+  <si>
+    <t>PLR: 0.9581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8451</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm4 &lt;- loadReg(wwTHg ~model(4), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm4</t>
+  </si>
+  <si>
+    <t>(Intercept)  -3.4872     0.9447 -3.6913  0.0004</t>
+  </si>
+  <si>
+    <t>lnQ           1.3486     0.1012 13.3210  0.0000</t>
+  </si>
+  <si>
+    <t>sin.DECTIME   0.7734     0.8190  0.9444  0.3183</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   1.5347     0.8031  1.9110  0.0481</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7744</t>
+  </si>
+  <si>
+    <t>R-squared: 89.07 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 75.26 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0388</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3931</t>
+  </si>
+  <si>
+    <t>lnQ         1.219</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 3.817</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 3.874</t>
+  </si>
+  <si>
+    <t>Est   0 0.03 0.47 2.51 5.02 5.57 6.11</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 7.17 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.072</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.866</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm5 &lt;- loadReg(wwTHg ~model(5), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm5</t>
+  </si>
+  <si>
+    <t>(Intercept)  -2.4071    0.24009 -10.026  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ           1.5264    0.09942  15.354  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2          0.1275    0.06894   1.849  0.0554</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.9174    0.36704  -2.499  0.0112</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.735</t>
+  </si>
+  <si>
+    <t>R-squared: 89.63 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 77.04 on 3 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9855</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.422</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.476</t>
+  </si>
+  <si>
+    <t>lnQ     1.239</t>
+  </si>
+  <si>
+    <t>lnQ2    1.130</t>
+  </si>
+  <si>
+    <t>DECTIME 1.368</t>
+  </si>
+  <si>
+    <t>Est   0 0.05 0.45 1.81 5.03 6.76 7.82</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.64 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8565</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm6 &lt;- loadReg(wwTHg ~model(6), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm6</t>
+  </si>
+  <si>
+    <t>(Intercept) -3.62956    1.01604 -3.5722  0.0004</t>
+  </si>
+  <si>
+    <t>lnQ          1.34667    0.10276 13.1044  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.03248    0.07725  0.4204  0.6495</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  0.87174    0.86273  1.0104  0.2781</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  1.53302    0.81436  1.8825  0.0477</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7963</t>
+  </si>
+  <si>
+    <t>R-squared: 89.13 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 75.47 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9671</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.0447</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4233</t>
+  </si>
+  <si>
+    <t>lnQ         1.222</t>
+  </si>
+  <si>
+    <t>lnQ2        1.309</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 4.119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Min  25%  50%  75%  90%  95% Max</t>
+  </si>
+  <si>
+    <t>Est   0 0.03 0.46 2.49 5.40 6.09 6.5</t>
+  </si>
+  <si>
+    <t>Obs   0 0.03 0.22 1.80 4.95 5.65 8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 11.33 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8572</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm7 &lt;- loadReg(wwTHg ~model(7), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm7</t>
+  </si>
+  <si>
+    <t>(Intercept)  -1.9025     1.1534 -1.6495  0.0808</t>
+  </si>
+  <si>
+    <t>lnQ           1.5354     0.1287 11.9279  0.0000</t>
+  </si>
+  <si>
+    <t>DECTIME      -0.9775     0.4514 -2.1653  0.0240</t>
+  </si>
+  <si>
+    <t>sin.DECTIME  -0.7279     1.0382 -0.7010  0.4497</t>
+  </si>
+  <si>
+    <t>cos.DECTIME   0.3797     0.9268  0.4097  0.6578</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.6896</t>
+  </si>
+  <si>
+    <t>R-squared: 90.59 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 80.35 on 4 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.5805</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.3689</t>
+  </si>
+  <si>
+    <t>lnQ         2.213</t>
+  </si>
+  <si>
+    <t>DECTIME     2.206</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.888</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.793</t>
+  </si>
+  <si>
+    <t>Est   0 0.03 0.56 2.21 3.79 6.60 7.47</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 0.2456 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8936</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm8 &lt;- loadReg(wwTHg ~model(8), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm8</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.05583    1.16824 -1.7598  0.0590</t>
+  </si>
+  <si>
+    <t>lnQ          1.54842    0.12982 11.9273  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.06803    0.07371  0.9229  0.3128</t>
+  </si>
+  <si>
+    <t>DECTIME     -1.06685    0.46283 -2.3051  0.0151</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.65915    1.04356 -0.6316  0.4880</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.27050    0.93664  0.2888  0.7505</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.6932</t>
+  </si>
+  <si>
+    <t>R-squared: 90.87 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 81.37 on 5 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.982</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.2737</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4219</t>
+  </si>
+  <si>
+    <t>lnQ         2.240</t>
+  </si>
+  <si>
+    <t>lnQ2        1.369</t>
+  </si>
+  <si>
+    <t>DECTIME     2.307</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 6.924</t>
+  </si>
+  <si>
+    <t>cos.DECTIME 5.887</t>
+  </si>
+  <si>
+    <t>Est   0 0.03 0.50 2.12 4.34 7.41 8.64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 7.97 percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.886</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm9 &lt;- loadReg(wwTHg ~model(9), data = wwTHg_Combined , flow="Flow", dates = "Dates" ,conc.units="ng/L" , station = "CCSB-Yolo")</t>
+  </si>
+  <si>
+    <t>&gt; wwTHg_Combinedm9</t>
+  </si>
+  <si>
+    <t>(Intercept) -2.10716    1.18748 -1.7745  0.0528</t>
+  </si>
+  <si>
+    <t>lnQ          1.49702    0.16336  9.1640  0.0000</t>
+  </si>
+  <si>
+    <t>lnQ2         0.07699    0.07657  1.0056  0.2635</t>
+  </si>
+  <si>
+    <t>DECTIME     -0.92739    0.53757 -1.7252  0.0594</t>
+  </si>
+  <si>
+    <t>DECTIME2    -1.32161    2.49150 -0.5304  0.5527</t>
+  </si>
+  <si>
+    <t>sin.DECTIME -0.28478    1.27114 -0.2240  0.8016</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  0.45233    1.00892  0.4483  0.6155</t>
+  </si>
+  <si>
+    <t>Residual variance: 0.7114</t>
+  </si>
+  <si>
+    <t>R-squared: 90.96 percent</t>
+  </si>
+  <si>
+    <t>G-squared: 81.73 on 6 degrees of freedom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  r = 0.9875</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  p-value = 0.5309</t>
+  </si>
+  <si>
+    <t>Serial Correlation of Residuals: 0.4133</t>
+  </si>
+  <si>
+    <t>lnQ          3.456</t>
+  </si>
+  <si>
+    <t>lnQ2         1.440</t>
+  </si>
+  <si>
+    <t>DECTIME      3.033</t>
+  </si>
+  <si>
+    <t>DECTIME2     1.943</t>
+  </si>
+  <si>
+    <t>sin.DECTIME 10.009</t>
+  </si>
+  <si>
+    <t>cos.DECTIME  6.656</t>
+  </si>
+  <si>
+    <t>Est   0 0.04 0.52 2.13 4.35 7.13 8.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bp: 7.646 percent</t>
+  </si>
+  <si>
+    <t>PLR: 1.076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  E: 0.8912</t>
+  </si>
+  <si>
+    <t>Number of Uncensored Observations: 34; Period of record: 2016-01-20 to 2017-04-26</t>
+  </si>
+  <si>
+    <t>x- Charlie</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2368,13 +2905,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2386,16 +2926,16 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3052,8 +3592,8 @@
   <dimension ref="A1:AI68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3067,10 +3607,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="42"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="6"/>
       <c r="K1" s="21" t="s">
         <v>21</v>
@@ -3109,24 +3649,24 @@
       <c r="L2" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="40"/>
+      <c r="O2" s="34"/>
     </row>
     <row r="3" spans="1:35" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
       <c r="Z4" s="18" t="s">
         <v>51</v>
       </c>
@@ -3141,21 +3681,21 @@
       <c r="AI4" s="18"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="32" t="s">
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="32"/>
+      <c r="L5" s="43"/>
       <c r="Z5" s="18" t="s">
         <v>52</v>
       </c>
@@ -3215,43 +3755,43 @@
       <c r="O6" s="1"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A7" s="11">
+      <c r="A7" s="6">
         <v>1</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="6">
         <v>0</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="6">
         <v>90.99</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="6">
         <v>0.21560000000000001</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="6">
         <v>9.8290000000000006</v>
       </c>
       <c r="L7" s="29">
         <v>0.81269999999999998</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="M7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N7" s="7" t="s">
@@ -3350,7 +3890,7 @@
         <v>0.85589999999999999</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>8</v>
+        <v>851</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>17</v>
@@ -3651,36 +4191,36 @@
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B18" s="33" t="s">
+      <c r="B18" s="40" t="s">
         <v>477</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="32" t="s">
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L18" s="32"/>
+      <c r="L18" s="43"/>
     </row>
     <row r="19" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -4165,36 +4705,36 @@
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="37" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B31" s="33" t="s">
+      <c r="B31" s="40" t="s">
         <v>672</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="32" t="s">
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L31" s="32"/>
+      <c r="L31" s="43"/>
     </row>
     <row r="32" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -4240,7 +4780,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <v>1</v>
       </c>
@@ -4284,11 +4824,11 @@
       <c r="P33" s="8" t="s">
         <v>479</v>
       </c>
-      <c r="AA33" s="9" t="s">
+      <c r="Y33" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="11">
         <v>2</v>
       </c>
@@ -4334,11 +4874,11 @@
       <c r="P34" s="8" t="s">
         <v>500</v>
       </c>
-      <c r="AA34" s="9" t="s">
+      <c r="Y34" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="29">
         <v>3</v>
       </c>
@@ -4382,11 +4922,11 @@
       <c r="P35" s="8" t="s">
         <v>517</v>
       </c>
-      <c r="AA35" s="9" t="s">
+      <c r="Y35" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>4</v>
       </c>
@@ -4430,11 +4970,11 @@
       <c r="P36" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="AA36" s="9" t="s">
+      <c r="Y36" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="11">
         <v>5</v>
       </c>
@@ -4480,11 +5020,11 @@
       <c r="P37" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="AA37" s="9" t="s">
+      <c r="Y37" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>6</v>
       </c>
@@ -4528,11 +5068,11 @@
       <c r="P38" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="AA38" s="9" t="s">
+      <c r="Y38" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A39" s="29">
         <v>7</v>
       </c>
@@ -4576,11 +5116,11 @@
       <c r="P39" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="AA39" s="9" t="s">
+      <c r="Y39" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>8</v>
       </c>
@@ -4624,11 +5164,11 @@
       <c r="P40" s="8" t="s">
         <v>623</v>
       </c>
-      <c r="AA40" s="9" t="s">
+      <c r="Y40" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A41" s="29">
         <v>9</v>
       </c>
@@ -4672,41 +5212,43 @@
       <c r="P41" s="8" t="s">
         <v>647</v>
       </c>
-      <c r="AA41" s="9" t="s">
+      <c r="Y41" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B43" s="36" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B43" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="37"/>
-      <c r="D43" s="37"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="37"/>
-      <c r="J43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B44" s="33"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="32" t="s">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B44" s="40" t="s">
+        <v>850</v>
+      </c>
+      <c r="C44" s="41"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="41"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L44" s="32"/>
-    </row>
-    <row r="45" spans="1:27" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="L44" s="43"/>
+    </row>
+    <row r="45" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>0</v>
       </c>
@@ -4750,36 +5292,46 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A46" s="29">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46" s="11">
         <v>1</v>
       </c>
       <c r="B46" s="11">
         <v>0</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="10" t="s">
+      <c r="D46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E46" s="10" t="s">
+      <c r="E46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="10" t="s">
+      <c r="F46" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G46" s="10" t="s">
+      <c r="G46" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
+      <c r="I46" s="11">
+        <v>87.07</v>
+      </c>
+      <c r="J46" s="11">
+        <v>0.4859</v>
+      </c>
+      <c r="K46" s="11">
+        <v>5.2969999999999997</v>
+      </c>
+      <c r="L46" s="32">
+        <v>0.87229999999999996</v>
+      </c>
+      <c r="M46" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N46" s="8" t="s">
         <v>17</v>
       </c>
@@ -4790,14 +5342,16 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A47" s="29">
         <v>2</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="6">
         <v>0</v>
       </c>
-      <c r="C47" s="25"/>
+      <c r="C47" s="25">
+        <v>0.30599999999999999</v>
+      </c>
       <c r="D47" s="10" t="s">
         <v>16</v>
       </c>
@@ -4810,13 +5364,21 @@
       <c r="G47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H47" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I47" s="29"/>
-      <c r="J47" s="29"/>
-      <c r="K47" s="29"/>
-      <c r="L47" s="29"/>
+      <c r="I47" s="32">
+        <v>87.46</v>
+      </c>
+      <c r="J47" s="32">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="K47" s="32">
+        <v>16.72</v>
+      </c>
+      <c r="L47" s="32">
+        <v>0.8468</v>
+      </c>
       <c r="M47" s="29"/>
       <c r="N47" s="8" t="s">
         <v>17</v>
@@ -4828,34 +5390,46 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A48" s="29">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" s="11">
         <v>3</v>
       </c>
       <c r="B48" s="11">
         <v>0</v>
       </c>
-      <c r="C48" s="10" t="s">
+      <c r="C48" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="E48" s="10" t="s">
+      <c r="D48" s="28">
+        <v>5.0900000000000001E-2</v>
+      </c>
+      <c r="E48" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H48" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I48" s="29"/>
-      <c r="J48" s="29"/>
-      <c r="K48" s="29"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="29"/>
+      <c r="I48" s="11">
+        <v>88.44</v>
+      </c>
+      <c r="J48" s="11">
+        <v>0.42870000000000003</v>
+      </c>
+      <c r="K48" s="11">
+        <v>-4.1879999999999997</v>
+      </c>
+      <c r="L48" s="32">
+        <v>0.84509999999999996</v>
+      </c>
+      <c r="M48" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N48" s="8" t="s">
         <v>17</v>
       </c>
@@ -4870,7 +5444,7 @@
       <c r="A49" s="29">
         <v>4</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="6">
         <v>0</v>
       </c>
       <c r="C49" s="10" t="s">
@@ -4882,15 +5456,27 @@
       <c r="E49" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F49" s="6"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="11" t="s">
+      <c r="F49" s="6">
+        <v>0.31830000000000003</v>
+      </c>
+      <c r="G49" s="32">
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I49" s="29"/>
-      <c r="J49" s="29"/>
-      <c r="K49" s="29"/>
-      <c r="L49" s="29"/>
+      <c r="I49" s="32">
+        <v>89.07</v>
+      </c>
+      <c r="J49" s="32">
+        <v>0.3931</v>
+      </c>
+      <c r="K49" s="32">
+        <v>7.17</v>
+      </c>
+      <c r="L49" s="32">
+        <v>0.86599999999999999</v>
+      </c>
       <c r="M49" s="29"/>
       <c r="N49" s="8" t="s">
         <v>17</v>
@@ -4903,31 +5489,45 @@
       </c>
     </row>
     <row r="50" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A50" s="29">
+      <c r="A50" s="11">
         <v>5</v>
       </c>
       <c r="B50" s="11">
         <v>0</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="10" t="s">
+      <c r="C50" s="11">
+        <v>5.5399999999999998E-2</v>
+      </c>
+      <c r="D50" s="11">
+        <v>1.12E-2</v>
+      </c>
+      <c r="E50" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F50" s="10" t="s">
+      <c r="F50" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G50" s="10" t="s">
+      <c r="G50" s="26" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
+      <c r="I50" s="11">
+        <v>89.63</v>
+      </c>
+      <c r="J50" s="11">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="K50" s="11">
+        <v>11.64</v>
+      </c>
+      <c r="L50" s="32">
+        <v>0.85650000000000004</v>
+      </c>
+      <c r="M50" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="N50" s="8" t="s">
         <v>17</v>
       </c>
@@ -4942,25 +5542,39 @@
       <c r="A51" s="29">
         <v>6</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="6">
         <v>0</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="32">
+        <v>0.64949999999999997</v>
+      </c>
       <c r="D51" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="6"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="11" t="s">
+      <c r="F51" s="6">
+        <v>0.27810000000000001</v>
+      </c>
+      <c r="G51" s="32">
+        <v>4.7699999999999999E-2</v>
+      </c>
+      <c r="H51" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I51" s="29"/>
-      <c r="J51" s="29"/>
-      <c r="K51" s="29"/>
-      <c r="L51" s="29"/>
+      <c r="I51" s="32">
+        <v>89.13</v>
+      </c>
+      <c r="J51" s="32">
+        <v>0.42330000000000001</v>
+      </c>
+      <c r="K51" s="32">
+        <v>11.33</v>
+      </c>
+      <c r="L51" s="32">
+        <v>0.85719999999999996</v>
+      </c>
       <c r="M51" s="29"/>
       <c r="N51" s="8" t="s">
         <v>17</v>
@@ -4976,25 +5590,39 @@
       <c r="A52" s="29">
         <v>7</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="6">
         <v>0</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6">
+        <v>2.4E-2</v>
+      </c>
       <c r="E52" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F52" s="6"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="11" t="s">
+      <c r="F52" s="6">
+        <v>0.44969999999999999</v>
+      </c>
+      <c r="G52" s="32">
+        <v>0.65780000000000005</v>
+      </c>
+      <c r="H52" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I52" s="29"/>
-      <c r="J52" s="29"/>
-      <c r="K52" s="29"/>
-      <c r="L52" s="29"/>
+      <c r="I52" s="32">
+        <v>90.59</v>
+      </c>
+      <c r="J52" s="32">
+        <v>0.36890000000000001</v>
+      </c>
+      <c r="K52" s="32">
+        <v>0.24560000000000001</v>
+      </c>
+      <c r="L52" s="32">
+        <v>0.89359999999999995</v>
+      </c>
       <c r="M52" s="29"/>
       <c r="N52" s="8" t="s">
         <v>17</v>
@@ -5010,23 +5638,39 @@
       <c r="A53" s="29">
         <v>8</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="6">
         <v>0</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="32">
+        <v>0.31280000000000002</v>
+      </c>
+      <c r="D53" s="6">
+        <v>1.5100000000000001E-2</v>
+      </c>
       <c r="E53" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="11" t="s">
+      <c r="F53" s="6">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0.75049999999999994</v>
+      </c>
+      <c r="H53" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I53" s="29"/>
-      <c r="J53" s="29"/>
-      <c r="K53" s="29"/>
-      <c r="L53" s="29"/>
+      <c r="I53" s="32">
+        <v>90.87</v>
+      </c>
+      <c r="J53" s="32">
+        <v>0.4219</v>
+      </c>
+      <c r="K53" s="32">
+        <v>7.97</v>
+      </c>
+      <c r="L53" s="32">
+        <v>0.88600000000000001</v>
+      </c>
       <c r="M53" s="29"/>
       <c r="N53" s="8" t="s">
         <v>17</v>
@@ -5042,21 +5686,39 @@
       <c r="A54" s="29">
         <v>9</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="6">
         <v>0</v>
       </c>
-      <c r="C54" s="29"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="11" t="s">
+      <c r="C54" s="32">
+        <v>0.26350000000000001</v>
+      </c>
+      <c r="D54" s="6">
+        <v>5.9400000000000001E-2</v>
+      </c>
+      <c r="E54" s="6">
+        <v>0.55269999999999997</v>
+      </c>
+      <c r="F54" s="6">
+        <v>0.80159999999999998</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0.61550000000000005</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I54" s="29"/>
-      <c r="J54" s="29"/>
-      <c r="K54" s="29"/>
-      <c r="L54" s="29"/>
+      <c r="I54" s="32">
+        <v>90.96</v>
+      </c>
+      <c r="J54" s="32">
+        <v>0.4133</v>
+      </c>
+      <c r="K54" s="32">
+        <v>7.6459999999999999</v>
+      </c>
+      <c r="L54" s="32">
+        <v>0.89119999999999999</v>
+      </c>
       <c r="M54" s="29"/>
       <c r="N54" s="8" t="s">
         <v>17</v>
@@ -5074,34 +5736,34 @@
       <c r="Y55" s="9"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C57" s="37"/>
-      <c r="D57" s="37"/>
-      <c r="E57" s="37"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="37"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="38"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="43"/>
+      <c r="L57" s="43"/>
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="B58" s="33"/>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="34"/>
-      <c r="G58" s="34"/>
-      <c r="H58" s="34"/>
-      <c r="I58" s="34"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="32" t="s">
+      <c r="B58" s="40"/>
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="42"/>
+      <c r="K58" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="L58" s="32"/>
+      <c r="L58" s="43"/>
     </row>
     <row r="59" spans="1:25" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
@@ -5341,12 +6003,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B4:J4"/>
-    <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="K5:L5"/>
     <mergeCell ref="K58:L58"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="B18:J18"/>
@@ -5359,6 +6015,12 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="K44:L44"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="B17:J17"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <conditionalFormatting sqref="L60:L68 L57 L93:L1048576">
     <cfRule type="cellIs" dxfId="29" priority="54" operator="between">
@@ -12908,115 +13570,173 @@
   <dimension ref="A1:A528"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T30" sqref="T30"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="15" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
+      <c r="A2" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="15" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="14" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="14" t="s">
+        <v>679</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="14" t="s">
+        <v>680</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
+      <c r="A27" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
+      <c r="A28" s="14" t="s">
+        <v>681</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="14" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="14" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="14" t="s">
+        <v>683</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="14" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="14" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="13"/>
@@ -13025,1465 +13745,2277 @@
       <c r="A37" s="13"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+      <c r="A39" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
+      <c r="A40" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="14" t="s">
+        <v>686</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="14" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="14" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="14" t="s">
+        <v>690</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="13"/>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="15" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
+      <c r="A53" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
+      <c r="A54" s="7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
+      <c r="A55" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="15" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="13"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="13"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="14"/>
+      <c r="A65" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="14"/>
+      <c r="A66" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="13"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="13"/>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="14" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="14" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="14" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="13"/>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
+      <c r="A79" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="14"/>
+      <c r="A80" s="14" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="14" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="14" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="14" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="14" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="14" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="13"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="14"/>
+      <c r="A90" s="14" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="14"/>
+      <c r="A91" s="14" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="14"/>
+      <c r="A92" s="14" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="13"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="14" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="14" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="14" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="14" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="13"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="15"/>
+      <c r="A108" s="15" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="7" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="15"/>
+      <c r="A112" s="15" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="13"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="13"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="13"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
+      <c r="A124" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
+      <c r="A125" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="13"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
+      <c r="A127" s="14" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="13"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
+      <c r="A129" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
+      <c r="A130" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
+      <c r="A131" s="14" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
+      <c r="A132" s="14" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
+      <c r="A133" s="14" t="s">
+        <v>710</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="13"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
+      <c r="A135" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
+      <c r="A136" s="14" t="s">
+        <v>711</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="14"/>
+      <c r="A137" s="14" t="s">
+        <v>712</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="14"/>
+      <c r="A138" s="14" t="s">
+        <v>713</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="14"/>
+      <c r="A139" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="14"/>
+      <c r="A140" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="14"/>
+      <c r="A141" s="14" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="14"/>
+      <c r="A142" s="14" t="s">
+        <v>715</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="14"/>
+      <c r="A143" s="14" t="s">
+        <v>716</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="13"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
+      <c r="A145" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="14"/>
+      <c r="A146" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="14"/>
+      <c r="A147" s="14" t="s">
+        <v>717</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="14"/>
+      <c r="A148" s="14" t="s">
+        <v>718</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="13"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="14"/>
+      <c r="A150" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="14"/>
+      <c r="A151" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="14"/>
+      <c r="A152" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="14"/>
+      <c r="A153" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="14"/>
+      <c r="A154" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="14"/>
+      <c r="A155" s="14" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="14"/>
+      <c r="A156" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" s="13"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="14"/>
+      <c r="A158" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="14"/>
+      <c r="A159" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="14"/>
+      <c r="A160" s="14" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="14"/>
+      <c r="A161" s="14" t="s">
+        <v>721</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="14"/>
+      <c r="A162" s="14" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" s="13"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="15"/>
+      <c r="A164" s="15" t="s">
+        <v>723</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="7"/>
+      <c r="A165" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="7"/>
+      <c r="A166" s="7" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="7"/>
+      <c r="A167" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="15"/>
+      <c r="A168" s="15" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="14"/>
+      <c r="A169" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" s="13"/>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="14"/>
+      <c r="A171" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="14"/>
+      <c r="A172" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" s="13"/>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="14"/>
+      <c r="A174" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="14"/>
+      <c r="A175" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="14"/>
+      <c r="A176" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="14"/>
+      <c r="A177" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="14"/>
+      <c r="A178" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="13"/>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="14"/>
+      <c r="A180" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="14"/>
+      <c r="A181" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" s="13"/>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A183" s="14"/>
+      <c r="A183" s="14" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" s="13"/>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A185" s="14"/>
+      <c r="A185" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A186" s="14"/>
+      <c r="A186" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A187" s="14"/>
+      <c r="A187" s="14" t="s">
+        <v>725</v>
+      </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A188" s="14"/>
+      <c r="A188" s="14" t="s">
+        <v>726</v>
+      </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A189" s="14"/>
+      <c r="A189" s="14" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A190" s="14"/>
+      <c r="A190" s="14" t="s">
+        <v>728</v>
+      </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" s="13"/>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A192" s="14"/>
+      <c r="A192" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A193" s="14"/>
+      <c r="A193" s="14" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A194" s="14"/>
+      <c r="A194" s="14" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A195" s="14"/>
+      <c r="A195" s="14" t="s">
+        <v>731</v>
+      </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A196" s="14"/>
+      <c r="A196" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A197" s="14"/>
+      <c r="A197" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A198" s="14"/>
+      <c r="A198" s="14" t="s">
+        <v>732</v>
+      </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A199" s="14"/>
+      <c r="A199" s="14" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A200" s="14"/>
+      <c r="A200" s="14" t="s">
+        <v>734</v>
+      </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="13"/>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A202" s="14"/>
+      <c r="A202" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A203" s="14"/>
+      <c r="A203" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A204" s="14"/>
+      <c r="A204" s="14" t="s">
+        <v>735</v>
+      </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A205" s="14"/>
+      <c r="A205" s="14" t="s">
+        <v>736</v>
+      </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A206" s="14"/>
+      <c r="A206" s="14" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" s="13"/>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A208" s="14"/>
+      <c r="A208" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A209" s="14"/>
+      <c r="A209" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A210" s="14"/>
+      <c r="A210" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A211" s="14"/>
+      <c r="A211" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A212" s="14"/>
+      <c r="A212" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A213" s="14"/>
+      <c r="A213" s="14" t="s">
+        <v>738</v>
+      </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A214" s="14"/>
+      <c r="A214" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A215" s="13"/>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A216" s="14"/>
+      <c r="A216" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A217" s="14"/>
+      <c r="A217" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A218" s="14"/>
+      <c r="A218" s="14" t="s">
+        <v>739</v>
+      </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A219" s="14"/>
+      <c r="A219" s="14" t="s">
+        <v>740</v>
+      </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A220" s="14"/>
+      <c r="A220" s="14" t="s">
+        <v>741</v>
+      </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A221" s="13"/>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A222" s="15"/>
+      <c r="A222" s="15" t="s">
+        <v>742</v>
+      </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A223" s="7"/>
+      <c r="A223" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A224" s="7"/>
+      <c r="A224" s="7" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A225" s="7"/>
+      <c r="A225" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A226" s="15"/>
+      <c r="A226" s="15" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A227" s="14"/>
+      <c r="A227" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A228" s="13"/>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A229" s="14"/>
+      <c r="A229" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A230" s="14"/>
+      <c r="A230" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A231" s="13"/>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A232" s="14"/>
+      <c r="A232" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A233" s="14"/>
+      <c r="A233" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A234" s="14"/>
+      <c r="A234" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A235" s="14"/>
+      <c r="A235" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A236" s="14"/>
+      <c r="A236" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A237" s="13"/>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A238" s="14"/>
+      <c r="A238" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A239" s="14"/>
+      <c r="A239" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A240" s="13"/>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A241" s="14"/>
+      <c r="A241" s="14" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A242" s="13"/>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A243" s="14"/>
+      <c r="A243" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A244" s="14"/>
+      <c r="A244" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A245" s="14"/>
+      <c r="A245" s="14" t="s">
+        <v>744</v>
+      </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A246" s="14"/>
+      <c r="A246" s="14" t="s">
+        <v>745</v>
+      </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A247" s="14"/>
+      <c r="A247" s="14" t="s">
+        <v>746</v>
+      </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A248" s="14"/>
+      <c r="A248" s="14" t="s">
+        <v>747</v>
+      </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A249" s="13"/>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A250" s="14"/>
+      <c r="A250" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A251" s="14"/>
+      <c r="A251" s="14" t="s">
+        <v>748</v>
+      </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A252" s="14"/>
+      <c r="A252" s="14" t="s">
+        <v>749</v>
+      </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A253" s="14"/>
+      <c r="A253" s="14" t="s">
+        <v>750</v>
+      </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A254" s="14"/>
+      <c r="A254" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A255" s="14"/>
+      <c r="A255" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A256" s="14"/>
+      <c r="A256" s="14" t="s">
+        <v>751</v>
+      </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A257" s="14"/>
+      <c r="A257" s="14" t="s">
+        <v>752</v>
+      </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A258" s="14"/>
+      <c r="A258" s="14" t="s">
+        <v>753</v>
+      </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A259" s="13"/>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A260" s="14"/>
+      <c r="A260" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A261" s="14"/>
+      <c r="A261" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A262" s="14"/>
+      <c r="A262" s="14" t="s">
+        <v>754</v>
+      </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A263" s="14"/>
+      <c r="A263" s="14" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A264" s="14"/>
+      <c r="A264" s="14" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A265" s="13"/>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A266" s="14"/>
+      <c r="A266" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A267" s="14"/>
+      <c r="A267" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A268" s="14"/>
+      <c r="A268" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A269" s="14"/>
+      <c r="A269" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A270" s="14"/>
+      <c r="A270" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A271" s="14"/>
+      <c r="A271" s="14" t="s">
+        <v>757</v>
+      </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A272" s="14"/>
+      <c r="A272" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A273" s="13"/>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A274" s="14"/>
+      <c r="A274" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A275" s="14"/>
+      <c r="A275" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A276" s="14"/>
+      <c r="A276" s="14" t="s">
+        <v>758</v>
+      </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A277" s="14"/>
+      <c r="A277" s="14" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A278" s="14"/>
+      <c r="A278" s="14" t="s">
+        <v>760</v>
+      </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A279" s="13"/>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A280" s="15"/>
+      <c r="A280" s="15" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A281" s="7"/>
+      <c r="A281" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A282" s="7"/>
+      <c r="A282" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A283" s="7"/>
+      <c r="A283" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A284" s="15"/>
+      <c r="A284" s="15" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A285" s="14"/>
+      <c r="A285" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A286" s="13"/>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A287" s="14"/>
+      <c r="A287" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A288" s="14"/>
+      <c r="A288" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A289" s="13"/>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A290" s="14"/>
+      <c r="A290" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A291" s="14"/>
+      <c r="A291" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A292" s="14"/>
+      <c r="A292" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A293" s="14"/>
+      <c r="A293" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A294" s="14"/>
+      <c r="A294" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A295" s="13"/>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A296" s="14"/>
+      <c r="A296" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A297" s="14"/>
+      <c r="A297" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A298" s="13"/>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A299" s="14"/>
+      <c r="A299" s="14" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A300" s="13"/>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A301" s="14"/>
+      <c r="A301" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="302" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A302" s="14"/>
+      <c r="A302" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="303" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A303" s="14"/>
+      <c r="A303" s="14" t="s">
+        <v>763</v>
+      </c>
     </row>
     <row r="304" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A304" s="14"/>
+      <c r="A304" s="14" t="s">
+        <v>764</v>
+      </c>
     </row>
     <row r="305" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A305" s="14"/>
+      <c r="A305" s="14" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="306" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A306" s="14"/>
+      <c r="A306" s="14" t="s">
+        <v>766</v>
+      </c>
     </row>
     <row r="307" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A307" s="14"/>
+      <c r="A307" s="14" t="s">
+        <v>767</v>
+      </c>
     </row>
     <row r="308" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A308" s="13"/>
     </row>
     <row r="309" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A309" s="14"/>
+      <c r="A309" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="310" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A310" s="14"/>
+      <c r="A310" s="14" t="s">
+        <v>768</v>
+      </c>
     </row>
     <row r="311" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A311" s="14"/>
+      <c r="A311" s="14" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="312" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A312" s="14"/>
+      <c r="A312" s="14" t="s">
+        <v>770</v>
+      </c>
     </row>
     <row r="313" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A313" s="14"/>
+      <c r="A313" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="314" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A314" s="14"/>
+      <c r="A314" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="315" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A315" s="14"/>
+      <c r="A315" s="14" t="s">
+        <v>771</v>
+      </c>
     </row>
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A316" s="14"/>
+      <c r="A316" s="14" t="s">
+        <v>772</v>
+      </c>
     </row>
     <row r="317" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A317" s="14"/>
+      <c r="A317" s="14" t="s">
+        <v>773</v>
+      </c>
     </row>
     <row r="318" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A318" s="13"/>
     </row>
     <row r="319" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A319" s="14"/>
+      <c r="A319" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="320" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A320" s="14"/>
+      <c r="A320" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="321" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A321" s="14"/>
+      <c r="A321" s="14" t="s">
+        <v>774</v>
+      </c>
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A322" s="14"/>
+      <c r="A322" s="14" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A323" s="14"/>
+      <c r="A323" s="14" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="324" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A324" s="14"/>
+      <c r="A324" s="14" t="s">
+        <v>737</v>
+      </c>
     </row>
     <row r="325" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A325" s="13"/>
     </row>
     <row r="326" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A326" s="14"/>
+      <c r="A326" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="327" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A327" s="14"/>
+      <c r="A327" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="328" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A328" s="14"/>
+      <c r="A328" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="329" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A329" s="14"/>
+      <c r="A329" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="330" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A330" s="14"/>
+      <c r="A330" s="14" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="331" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A331" s="14"/>
+      <c r="A331" s="14" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="332" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A332" s="14"/>
+      <c r="A332" s="14" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="333" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A333" s="13"/>
     </row>
     <row r="334" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A334" s="14"/>
+      <c r="A334" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="335" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A335" s="14"/>
+      <c r="A335" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="336" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A336" s="14"/>
+      <c r="A336" s="14" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="337" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A337" s="14"/>
+      <c r="A337" s="14" t="s">
+        <v>781</v>
+      </c>
     </row>
     <row r="338" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A338" s="14"/>
+      <c r="A338" s="14" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="339" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A339" s="13"/>
     </row>
     <row r="340" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A340" s="15"/>
+      <c r="A340" s="15" t="s">
+        <v>783</v>
+      </c>
     </row>
     <row r="341" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A341" s="7"/>
+      <c r="A341" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="342" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A342" s="7"/>
+      <c r="A342" s="7" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="343" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A343" s="7"/>
+      <c r="A343" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="344" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A344" s="15"/>
+      <c r="A344" s="15" t="s">
+        <v>784</v>
+      </c>
     </row>
     <row r="345" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A345" s="14"/>
+      <c r="A345" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="346" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A346" s="13"/>
     </row>
     <row r="347" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A347" s="14"/>
+      <c r="A347" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="348" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A348" s="14"/>
+      <c r="A348" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="349" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A349" s="13"/>
     </row>
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A350" s="14"/>
+      <c r="A350" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="351" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A351" s="14"/>
+      <c r="A351" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="352" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A352" s="14"/>
+      <c r="A352" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A353" s="14"/>
+      <c r="A353" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A354" s="14"/>
+      <c r="A354" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A355" s="13"/>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A356" s="14"/>
+      <c r="A356" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A357" s="14"/>
+      <c r="A357" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="358" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A358" s="13"/>
     </row>
     <row r="359" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A359" s="14"/>
+      <c r="A359" s="14" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="360" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A360" s="13"/>
     </row>
     <row r="361" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A361" s="14"/>
+      <c r="A361" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="362" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A362" s="14"/>
+      <c r="A362" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A363" s="14"/>
+      <c r="A363" s="14" t="s">
+        <v>785</v>
+      </c>
     </row>
     <row r="364" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A364" s="14"/>
+      <c r="A364" s="14" t="s">
+        <v>786</v>
+      </c>
     </row>
     <row r="365" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A365" s="14"/>
+      <c r="A365" s="14" t="s">
+        <v>787</v>
+      </c>
     </row>
     <row r="366" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A366" s="14"/>
+      <c r="A366" s="14" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="367" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A367" s="14"/>
+      <c r="A367" s="14" t="s">
+        <v>789</v>
+      </c>
     </row>
     <row r="368" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A368" s="13"/>
     </row>
     <row r="369" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A369" s="14"/>
+      <c r="A369" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="370" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A370" s="14"/>
+      <c r="A370" s="14" t="s">
+        <v>790</v>
+      </c>
     </row>
     <row r="371" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A371" s="14"/>
+      <c r="A371" s="14" t="s">
+        <v>791</v>
+      </c>
     </row>
     <row r="372" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A372" s="14"/>
+      <c r="A372" s="14" t="s">
+        <v>792</v>
+      </c>
     </row>
     <row r="373" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A373" s="14"/>
+      <c r="A373" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="374" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A374" s="14"/>
+      <c r="A374" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="375" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A375" s="14"/>
+      <c r="A375" s="14" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="376" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A376" s="14"/>
+      <c r="A376" s="14" t="s">
+        <v>793</v>
+      </c>
     </row>
     <row r="377" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A377" s="14"/>
+      <c r="A377" s="14" t="s">
+        <v>794</v>
+      </c>
     </row>
     <row r="378" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A378" s="13"/>
     </row>
     <row r="379" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A379" s="14"/>
+      <c r="A379" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="380" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A380" s="14"/>
+      <c r="A380" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="381" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A381" s="14"/>
+      <c r="A381" s="14" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="382" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A382" s="14"/>
+      <c r="A382" s="14" t="s">
+        <v>796</v>
+      </c>
     </row>
     <row r="383" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A383" s="14"/>
+      <c r="A383" s="14" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="384" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A384" s="14"/>
+      <c r="A384" s="14" t="s">
+        <v>798</v>
+      </c>
     </row>
     <row r="385" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A385" s="13"/>
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A386" s="14"/>
+      <c r="A386" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="387" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A387" s="14"/>
+      <c r="A387" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="388" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A388" s="14"/>
+      <c r="A388" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="389" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A389" s="14"/>
+      <c r="A389" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="390" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A390" s="14"/>
+      <c r="A390" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="391" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A391" s="14"/>
+      <c r="A391" s="14" t="s">
+        <v>799</v>
+      </c>
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A392" s="14"/>
+      <c r="A392" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A393" s="13"/>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A394" s="14"/>
+      <c r="A394" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A395" s="14"/>
+      <c r="A395" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A396" s="14"/>
+      <c r="A396" s="14" t="s">
+        <v>800</v>
+      </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A397" s="14"/>
+      <c r="A397" s="14" t="s">
+        <v>801</v>
+      </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A398" s="14"/>
+      <c r="A398" s="14" t="s">
+        <v>802</v>
+      </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A399" s="13"/>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A400" s="15"/>
+      <c r="A400" s="15" t="s">
+        <v>803</v>
+      </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A401" s="7"/>
+      <c r="A401" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A402" s="7"/>
+      <c r="A402" s="7" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A403" s="7"/>
+      <c r="A403" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A404" s="15"/>
+      <c r="A404" s="15" t="s">
+        <v>804</v>
+      </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A405" s="14"/>
+      <c r="A405" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A406" s="13"/>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A407" s="14"/>
+      <c r="A407" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A408" s="14"/>
+      <c r="A408" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A409" s="13"/>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A410" s="14"/>
+      <c r="A410" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A411" s="14"/>
+      <c r="A411" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A412" s="14"/>
+      <c r="A412" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A413" s="14"/>
+      <c r="A413" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A414" s="14"/>
+      <c r="A414" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A415" s="13"/>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A416" s="14"/>
+      <c r="A416" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A417" s="14"/>
+      <c r="A417" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A418" s="13"/>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A419" s="14"/>
+      <c r="A419" s="14" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A420" s="13"/>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A421" s="14"/>
+      <c r="A421" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A422" s="14"/>
+      <c r="A422" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A423" s="14"/>
+      <c r="A423" s="14" t="s">
+        <v>805</v>
+      </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A424" s="14"/>
+      <c r="A424" s="14" t="s">
+        <v>806</v>
+      </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A425" s="14"/>
+      <c r="A425" s="14" t="s">
+        <v>807</v>
+      </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A426" s="14"/>
+      <c r="A426" s="14" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A427" s="14"/>
+      <c r="A427" s="14" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A428" s="14"/>
+      <c r="A428" s="14" t="s">
+        <v>810</v>
+      </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A429" s="13"/>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A430" s="14"/>
+      <c r="A430" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A431" s="14"/>
+      <c r="A431" s="14" t="s">
+        <v>811</v>
+      </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
+      <c r="A432" s="14" t="s">
+        <v>812</v>
+      </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
+      <c r="A433" s="14" t="s">
+        <v>813</v>
+      </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
+      <c r="A434" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
+      <c r="A435" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
+      <c r="A436" s="14" t="s">
+        <v>814</v>
+      </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A437" s="14"/>
+      <c r="A437" s="14" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A438" s="14"/>
+      <c r="A438" s="14" t="s">
+        <v>816</v>
+      </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A439" s="13"/>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A440" s="14"/>
+      <c r="A440" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
+      <c r="A441" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A442" s="14"/>
+      <c r="A442" s="14" t="s">
+        <v>817</v>
+      </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A443" s="14"/>
+      <c r="A443" s="14" t="s">
+        <v>818</v>
+      </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A444" s="14"/>
+      <c r="A444" s="14" t="s">
+        <v>819</v>
+      </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
+      <c r="A445" s="14" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
+      <c r="A446" s="14" t="s">
+        <v>821</v>
+      </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A447" s="13"/>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
+      <c r="A448" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
+      <c r="A449" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A450" s="14"/>
+      <c r="A450" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A451" s="14"/>
+      <c r="A451" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A452" s="14"/>
+      <c r="A452" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A453" s="14"/>
+      <c r="A453" s="14" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A454" s="14"/>
+      <c r="A454" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A455" s="13"/>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A456" s="14"/>
+      <c r="A456" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A457" s="14"/>
+      <c r="A457" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
+      <c r="A458" s="14" t="s">
+        <v>823</v>
+      </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
+      <c r="A459" s="14" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A460" s="14"/>
+      <c r="A460" s="14" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A461" s="13"/>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A462" s="15"/>
+      <c r="A462" s="15" t="s">
+        <v>825</v>
+      </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A463" s="7"/>
+      <c r="A463" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A464" s="7"/>
+      <c r="A464" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A465" s="7"/>
+      <c r="A465" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A466" s="15"/>
+      <c r="A466" s="15" t="s">
+        <v>826</v>
+      </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A467" s="14"/>
+      <c r="A467" s="14" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A468" s="13"/>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A469" s="14"/>
+      <c r="A469" s="14" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A470" s="14"/>
+      <c r="A470" s="14" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A471" s="13"/>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A472" s="14"/>
+      <c r="A472" s="14" t="s">
+        <v>675</v>
+      </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A473" s="14"/>
+      <c r="A473" s="14" t="s">
+        <v>676</v>
+      </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A474" s="14"/>
+      <c r="A474" s="14" t="s">
+        <v>677</v>
+      </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A475" s="14"/>
+      <c r="A475" s="14" t="s">
+        <v>678</v>
+      </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A476" s="14"/>
+      <c r="A476" s="14" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A477" s="13"/>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A478" s="14"/>
+      <c r="A478" s="14" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A479" s="14"/>
+      <c r="A479" s="14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A480" s="13"/>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A481" s="14"/>
+      <c r="A481" s="14" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A482" s="13"/>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A483" s="14"/>
+      <c r="A483" s="14" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A484" s="14"/>
+      <c r="A484" s="14" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A485" s="14"/>
+      <c r="A485" s="14" t="s">
+        <v>827</v>
+      </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A486" s="14"/>
+      <c r="A486" s="14" t="s">
+        <v>828</v>
+      </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A487" s="14"/>
+      <c r="A487" s="14" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A488" s="14"/>
+      <c r="A488" s="14" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A489" s="14"/>
+      <c r="A489" s="14" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A490" s="14"/>
+      <c r="A490" s="14" t="s">
+        <v>832</v>
+      </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A491" s="14"/>
+      <c r="A491" s="14" t="s">
+        <v>833</v>
+      </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A492" s="13"/>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A493" s="14"/>
+      <c r="A493" s="14" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A494" s="14"/>
+      <c r="A494" s="14" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A495" s="14"/>
+      <c r="A495" s="14" t="s">
+        <v>835</v>
+      </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A496" s="14"/>
+      <c r="A496" s="14" t="s">
+        <v>836</v>
+      </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A497" s="14"/>
+      <c r="A497" s="14" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A498" s="14"/>
+      <c r="A498" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A499" s="14"/>
+      <c r="A499" s="14" t="s">
+        <v>837</v>
+      </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A500" s="14"/>
+      <c r="A500" s="14" t="s">
+        <v>838</v>
+      </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A501" s="14"/>
+      <c r="A501" s="14" t="s">
+        <v>839</v>
+      </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A502" s="13"/>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A503" s="14"/>
+      <c r="A503" s="14" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A504" s="14"/>
+      <c r="A504" s="14" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A505" s="14"/>
+      <c r="A505" s="14" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A506" s="14"/>
+      <c r="A506" s="14" t="s">
+        <v>841</v>
+      </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A507" s="14"/>
+      <c r="A507" s="14" t="s">
+        <v>842</v>
+      </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A508" s="14"/>
+      <c r="A508" s="14" t="s">
+        <v>843</v>
+      </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A509" s="14"/>
+      <c r="A509" s="14" t="s">
+        <v>844</v>
+      </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A510" s="14"/>
+      <c r="A510" s="14" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A511" s="13"/>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A512" s="14"/>
+      <c r="A512" s="14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A513" s="14"/>
+      <c r="A513" s="14" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A514" s="14"/>
+      <c r="A514" s="14" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A515" s="14"/>
+      <c r="A515" s="14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A516" s="14"/>
+      <c r="A516" s="14" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A517" s="14"/>
+      <c r="A517" s="14" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A518" s="14"/>
+      <c r="A518" s="14" t="s">
+        <v>687</v>
+      </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A519" s="13"/>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A520" s="14"/>
+      <c r="A520" s="14" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A521" s="14"/>
+      <c r="A521" s="14" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A522" s="14"/>
+      <c r="A522" s="14" t="s">
+        <v>847</v>
+      </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A523" s="14"/>
+      <c r="A523" s="14" t="s">
+        <v>848</v>
+      </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A524" s="14"/>
+      <c r="A524" s="14" t="s">
+        <v>849</v>
+      </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A525" s="16"/>

</xml_diff>